<commit_message>
Added Conditional Formatting and Filters
</commit_message>
<xml_diff>
--- a/PRACTICE AND LEARNING.xlsx
+++ b/PRACTICE AND LEARNING.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C4D51F-C35C-4254-940A-60F952C8AEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E537B97F-3CAE-4FBE-89BF-13A3CF1956BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F342A09-57DA-43F0-A74F-9FCC3C63F038}"/>
   </bookViews>
   <sheets>
     <sheet name="PRACTICE SHEET 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PRACTICE SHEET 1'!$A$3:$L$13</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -322,6 +325,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -331,9 +337,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,7 +659,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,20 +678,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -762,366 +765,383 @@
         <f>AVERAGE(E4,F4,G4,H4)</f>
         <v>78.5</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="11">
         <f>I4/J4*100</f>
         <v>89.714285714285708</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3">
-        <v>36267</v>
+        <v>36270</v>
       </c>
       <c r="E5" s="2">
         <v>83</v>
       </c>
       <c r="F5" s="2">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G5" s="2">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="H5" s="2">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ref="I5:I13" si="0">SUM(E5,F5,G5,H5)</f>
-        <v>294</v>
+        <f>SUM(E5,F5,G5,H5)</f>
+        <v>304</v>
       </c>
       <c r="J5" s="2">
         <v>350</v>
       </c>
       <c r="K5" s="10">
-        <f t="shared" ref="K5:K13" si="1">AVERAGE(E5,F5,G5,H5)</f>
-        <v>73.5</v>
-      </c>
-      <c r="L5" s="14">
-        <f t="shared" ref="L5:L13" si="2">I5/J5*100</f>
-        <v>84</v>
+        <f>AVERAGE(E5,F5,G5,H5)</f>
+        <v>76</v>
+      </c>
+      <c r="L5" s="11">
+        <f>I5/J5*100</f>
+        <v>86.857142857142861</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3">
-        <v>37146</v>
+        <v>37374</v>
       </c>
       <c r="E6" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F6" s="2">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G6" s="2">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H6" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="0"/>
-        <v>284</v>
+        <f>SUM(E6,F6,G6,H6)</f>
+        <v>298</v>
       </c>
       <c r="J6" s="2">
         <v>350</v>
       </c>
       <c r="K6" s="10">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="L6" s="14">
-        <f t="shared" si="2"/>
-        <v>81.142857142857139</v>
+        <f>AVERAGE(E6,F6,G6,H6)</f>
+        <v>74.5</v>
+      </c>
+      <c r="L6" s="11">
+        <f>I6/J6*100</f>
+        <v>85.142857142857139</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3">
-        <v>36856</v>
+        <v>36267</v>
       </c>
       <c r="E7" s="2">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F7" s="2">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G7" s="2">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H7" s="2">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="0"/>
-        <v>293</v>
+        <f>SUM(E7,F7,G7,H7)</f>
+        <v>294</v>
       </c>
       <c r="J7" s="2">
         <v>350</v>
       </c>
       <c r="K7" s="10">
-        <f t="shared" si="1"/>
-        <v>73.25</v>
-      </c>
-      <c r="L7" s="14">
-        <f t="shared" si="2"/>
-        <v>83.714285714285722</v>
+        <f>AVERAGE(E7,F7,G7,H7)</f>
+        <v>73.5</v>
+      </c>
+      <c r="L7" s="11">
+        <f>I7/J7*100</f>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="3">
-        <v>36688</v>
+        <v>36856</v>
       </c>
       <c r="E8" s="2">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F8" s="2">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="G8" s="2">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H8" s="2">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="0"/>
-        <v>276</v>
+        <f>SUM(E8,F8,G8,H8)</f>
+        <v>293</v>
       </c>
       <c r="J8" s="2">
         <v>350</v>
       </c>
       <c r="K8" s="10">
-        <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="L8" s="14">
-        <f t="shared" si="2"/>
-        <v>78.857142857142861</v>
+        <f>AVERAGE(E8,F8,G8,H8)</f>
+        <v>73.25</v>
+      </c>
+      <c r="L8" s="11">
+        <f>I8/J8*100</f>
+        <v>83.714285714285722</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="3">
-        <v>36266</v>
+        <v>36787</v>
       </c>
       <c r="E9" s="2">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F9" s="2">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="G9" s="2">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H9" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="0"/>
-        <v>289</v>
+        <f>SUM(E9,F9,G9,H9)</f>
+        <v>292</v>
       </c>
       <c r="J9" s="2">
         <v>350</v>
       </c>
       <c r="K9" s="10">
-        <f t="shared" si="1"/>
-        <v>72.25</v>
-      </c>
-      <c r="L9" s="14">
-        <f t="shared" si="2"/>
-        <v>82.571428571428569</v>
+        <f>AVERAGE(E9,F9,G9,H9)</f>
+        <v>73</v>
+      </c>
+      <c r="L9" s="11">
+        <f>I9/J9*100</f>
+        <v>83.428571428571431</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3">
-        <v>36787</v>
+        <v>36266</v>
       </c>
       <c r="E10" s="2">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F10" s="2">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G10" s="2">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H10" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="0"/>
-        <v>292</v>
+        <f>SUM(E10,F10,G10,H10)</f>
+        <v>289</v>
       </c>
       <c r="J10" s="2">
         <v>350</v>
       </c>
       <c r="K10" s="10">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="L10" s="14">
-        <f t="shared" si="2"/>
-        <v>83.428571428571431</v>
+        <f>AVERAGE(E10,F10,G10,H10)</f>
+        <v>72.25</v>
+      </c>
+      <c r="L10" s="11">
+        <f>I10/J10*100</f>
+        <v>82.571428571428569</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3">
-        <v>36270</v>
+        <v>37146</v>
       </c>
       <c r="E11" s="2">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F11" s="2">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G11" s="2">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="H11" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="0"/>
-        <v>304</v>
+        <f>SUM(E11,F11,G11,H11)</f>
+        <v>284</v>
       </c>
       <c r="J11" s="2">
         <v>350</v>
       </c>
       <c r="K11" s="10">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="L11" s="14">
-        <f t="shared" si="2"/>
-        <v>86.857142857142861</v>
+        <f>AVERAGE(E11,F11,G11,H11)</f>
+        <v>71</v>
+      </c>
+      <c r="L11" s="11">
+        <f>I11/J11*100</f>
+        <v>81.142857142857139</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3">
-        <v>36891</v>
+        <v>36688</v>
       </c>
       <c r="E12" s="2">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F12" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G12" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H12" s="2">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="0"/>
-        <v>275</v>
+        <f>SUM(E12,F12,G12,H12)</f>
+        <v>276</v>
       </c>
       <c r="J12" s="2">
         <v>350</v>
       </c>
       <c r="K12" s="10">
-        <f t="shared" si="1"/>
-        <v>68.75</v>
-      </c>
-      <c r="L12" s="14">
-        <f t="shared" si="2"/>
-        <v>78.571428571428569</v>
+        <f>AVERAGE(E12,F12,G12,H12)</f>
+        <v>69</v>
+      </c>
+      <c r="L12" s="11">
+        <f>I12/J12*100</f>
+        <v>78.857142857142861</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9">
-        <v>37374</v>
+        <v>36891</v>
       </c>
       <c r="E13" s="8">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F13" s="8">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="G13" s="8">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H13" s="8">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I13" s="8">
-        <f t="shared" si="0"/>
-        <v>298</v>
+        <f>SUM(E13,F13,G13,H13)</f>
+        <v>275</v>
       </c>
       <c r="J13" s="8">
         <v>350</v>
       </c>
-      <c r="K13" s="15">
-        <f t="shared" si="1"/>
-        <v>74.5</v>
-      </c>
-      <c r="L13" s="16">
-        <f t="shared" si="2"/>
-        <v>85.142857142857139</v>
+      <c r="K13" s="12">
+        <f>AVERAGE(E13,F13,G13,H13)</f>
+        <v>68.75</v>
+      </c>
+      <c r="L13" s="13">
+        <f>I13/J13*100</f>
+        <v>78.571428571428569</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:L13" xr:uid="{FE02FB22-650F-4F0D-8477-938CAC2CDB59}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L13">
+      <sortCondition descending="1" ref="I3:I13"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A2:L2"/>
   </mergeCells>
+  <conditionalFormatting sqref="E4:E13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhanced Visualization for Percentage and Obtained Marks
</commit_message>
<xml_diff>
--- a/PRACTICE AND LEARNING.xlsx
+++ b/PRACTICE AND LEARNING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E537B97F-3CAE-4FBE-89BF-13A3CF1956BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FB416F-EB1E-4E47-BD1B-63C2A34161C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F342A09-57DA-43F0-A74F-9FCC3C63F038}"/>
   </bookViews>
@@ -659,7 +659,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,6 +1131,30 @@
     <mergeCell ref="A2:L2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I13">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>